<commit_message>
Add argument to pass partner short name variable from PDF extraction to BPA translator to obtain Oracle name.
</commit_message>
<xml_diff>
--- a/Data/Input/Test_Quote.xlsx
+++ b/Data/Input/Test_Quote.xlsx
@@ -7,6 +7,7 @@
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Shub" sheetId="2" r:id="rId2"/>
+    <x:sheet name="CmQuote" sheetId="5" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="137">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
   <x:si>
     <x:t>Item Description</x:t>
   </x:si>
@@ -426,6 +427,27 @@
   <x:si>
     <x:t>Units ISP Fiber Deployment- Estate Acquisition Gated Community clusters (over 2000 Units )</x:t>
   </x:si>
+  <x:si>
+    <x:t>Costs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Service Costs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ksh 276,804.52</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Material costs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ksh 52,258.40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Total Excluding VAT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ksh 329,062.92</x:t>
+  </x:si>
 </x:sst>
 </file>
 
@@ -29996,4 +30018,59 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:C4"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:3">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3">
+      <x:c r="A2" s="0" t="s">
+        <x:v>138</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>139</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="A3" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
+      <x:c r="A4" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
Pull in Data Entry Workflow to test variables transfer via arguments
</commit_message>
<xml_diff>
--- a/Data/Input/Test_Quote.xlsx
+++ b/Data/Input/Test_Quote.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="144">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
   <x:si>
     <x:t>Item Description</x:t>
   </x:si>
@@ -428,25 +428,133 @@
     <x:t>Units ISP Fiber Deployment- Estate Acquisition Gated Community clusters (over 2000 Units )</x:t>
   </x:si>
   <x:si>
-    <x:t>Costs</x:t>
+    <x:t>Installation of Aerial Cable</x:t>
   </x:si>
   <x:si>
-    <x:t>Service Costs</x:t>
+    <x:t>43.00</x:t>
   </x:si>
   <x:si>
-    <x:t>Ksh 276,804.52</x:t>
+    <x:t>510</x:t>
   </x:si>
   <x:si>
-    <x:t>Material costs</x:t>
+    <x:t>21,930.00</x:t>
   </x:si>
   <x:si>
-    <x:t>Ksh 52,258.40</x:t>
+    <x:t>As built documents</x:t>
   </x:si>
   <x:si>
-    <x:t>Total Excluding VAT</x:t>
+    <x:t>5.28</x:t>
   </x:si>
   <x:si>
-    <x:t>Ksh 329,062.92</x:t>
+    <x:t>397</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2,096.16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Field detailed survey report</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6,352.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Project Management Aerial Incl of H&amp;S per meter</x:t>
+  </x:si>
+  <x:si>
+    <x:t>47.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>18,659.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pole Cable Bracket, Supply and Installation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2,200.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pole Down-lead clamp, Supply and Installation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1,500.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4,500.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pole Support, Supply and Installation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9,000.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27,000.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pole, Supply &amp; installation Wooden 10m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13,500.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>54,000.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pole Tangent Support, Supply and Installation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1,800.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pole, Supply &amp; installation Wooden 8m</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11,000.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>55,000.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Supply and installation of Universal Pole bracket</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1,250.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7,500.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Pole Tension Clamp, Supply and Installation</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2,300.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>27,600.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Splicing, Testing and Commissioning 1 Core</x:t>
+  </x:si>
+  <x:si>
+    <x:t>440.00</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -30031,39 +30139,310 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:3">
+    <x:row r="1" spans="1:5">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5">
+      <x:c r="A2" s="0" t="s">
         <x:v>137</x:v>
       </x:c>
-      <x:c r="C1" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="2" spans="1:3">
-      <x:c r="A2" s="0" t="s">
+      <x:c r="B2" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
         <x:v>138</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="D2" s="0" t="s">
         <x:v>139</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:3">
+      <x:c r="E2" s="0" t="s">
+        <x:v>140</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5">
       <x:c r="A3" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:5">
+      <x:c r="A4" s="0" t="s">
         <x:v>141</x:v>
       </x:c>
-    </x:row>
-    <x:row r="4" spans="1:3">
-      <x:c r="A4" s="0" t="s">
+      <x:c r="B4" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
         <x:v>142</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s">
+      <x:c r="D4" s="0" t="s">
         <x:v>143</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>144</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:5">
+      <x:c r="A5" s="0" t="s">
+        <x:v>145</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>146</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>147</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:5">
+      <x:c r="A6" s="0" t="s">
+        <x:v>148</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>149</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>150</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:5">
+      <x:c r="A7" s="0" t="s">
+        <x:v>151</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>152</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:5">
+      <x:c r="A8" s="0" t="s">
+        <x:v>154</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>155</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>156</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:5">
+      <x:c r="A9" s="0" t="s">
+        <x:v>157</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>159</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:5">
+      <x:c r="A10" s="0" t="s">
+        <x:v>160</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>161</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>163</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:5">
+      <x:c r="A11" s="0" t="s">
+        <x:v>164</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>165</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>166</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>158</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:5">
+      <x:c r="A12" s="0" t="s">
+        <x:v>167</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>168</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>166</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>169</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:5">
+      <x:c r="A13" s="0" t="s">
+        <x:v>170</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>171</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>172</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>173</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:5">
+      <x:c r="A14" s="0" t="s">
+        <x:v>174</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>175</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>176</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>177</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:5">
+      <x:c r="A15" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:5">
+      <x:c r="A16" s="0" t="s">
+        <x:v>96</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>97</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:5">
+      <x:c r="A17" s="0" t="s">
+        <x:v>129</x:v>
+      </x:c>
+      <x:c r="B17" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C17" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+      <x:c r="D17" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="E17" s="0" t="s">
+        <x:v>130</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:5">
+      <x:c r="A18" s="0" t="s">
+        <x:v>178</x:v>
+      </x:c>
+      <x:c r="B18" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C18" s="0" t="s">
+        <x:v>179</x:v>
+      </x:c>
+      <x:c r="D18" s="0" t="s">
+        <x:v>153</x:v>
+      </x:c>
+      <x:c r="E18" s="0" t="s">
+        <x:v>55</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Update Oracle Supplier name on CMQuote
</commit_message>
<xml_diff>
--- a/Data/Input/Test_Quote.xlsx
+++ b/Data/Input/Test_Quote.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="180">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
   <x:si>
     <x:t>Item Description</x:t>
   </x:si>
@@ -428,10 +428,13 @@
     <x:t>Units ISP Fiber Deployment- Estate Acquisition Gated Community clusters (over 2000 Units )</x:t>
   </x:si>
   <x:si>
-    <x:t>Installation of Aerial Cable</x:t>
+    <x:t>Costs</x:t>
   </x:si>
   <x:si>
-    <x:t>43.00</x:t>
+    <x:t>Service Costs</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ksh 276,804.52</x:t>
   </x:si>
   <x:si>
     <x:t>510</x:t>
@@ -440,10 +443,16 @@
     <x:t>21,930.00</x:t>
   </x:si>
   <x:si>
-    <x:t>As built documents</x:t>
+    <x:t>Material costs</x:t>
   </x:si>
   <x:si>
-    <x:t>5.28</x:t>
+    <x:t>Ksh 52,258.40</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Total Excluding VAT</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ksh 329,062.92</x:t>
   </x:si>
   <x:si>
     <x:t>397</x:t>
@@ -30144,10 +30153,10 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>137</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>2</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
         <x:v>3</x:v>
@@ -30158,30 +30167,24 @@
     </x:row>
     <x:row r="2" spans="1:5">
       <x:c r="A2" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>138</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="s">
-        <x:v>138</x:v>
+        <x:v>139</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>139</x:v>
+        <x:v>140</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>140</x:v>
+        <x:v>141</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5">
       <x:c r="A3" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>142</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>49</x:v>
@@ -30192,67 +30195,64 @@
     </x:row>
     <x:row r="4" spans="1:5">
       <x:c r="A4" s="0" t="s">
-        <x:v>141</x:v>
+        <x:v>144</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>145</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>144</x:v>
+        <x:v>147</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5">
       <x:c r="A5" s="0" t="s">
-        <x:v>145</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
+        <x:v>149</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
         <x:v>146</x:v>
       </x:c>
-      <x:c r="D5" s="0" t="s">
-        <x:v>143</x:v>
-      </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>147</x:v>
+        <x:v>150</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:5">
       <x:c r="A6" s="0" t="s">
-        <x:v>148</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>150</x:v>
+        <x:v>153</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:5">
       <x:c r="A7" s="0" t="s">
-        <x:v>151</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
         <x:v>97</x:v>
@@ -30260,121 +30260,121 @@
     </x:row>
     <x:row r="8" spans="1:5">
       <x:c r="A8" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
         <x:v>60</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>156</x:v>
+        <x:v>159</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:5">
       <x:c r="A9" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>161</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
         <x:v>60</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>159</x:v>
+        <x:v>162</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:5">
       <x:c r="A10" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>163</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>164</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>162</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>166</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:5">
       <x:c r="A11" s="0" t="s">
-        <x:v>164</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>165</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>161</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:5">
       <x:c r="A12" s="0" t="s">
-        <x:v>167</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>168</x:v>
+        <x:v>171</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>166</x:v>
+        <x:v>169</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>172</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:5">
       <x:c r="A13" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>173</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>171</x:v>
+        <x:v>174</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>172</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>173</x:v>
+        <x:v>176</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:5">
       <x:c r="A14" s="0" t="s">
-        <x:v>174</x:v>
+        <x:v>177</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>175</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>176</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>177</x:v>
+        <x:v>180</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:5">
@@ -30430,16 +30430,16 @@
     </x:row>
     <x:row r="18" spans="1:5">
       <x:c r="A18" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>181</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>182</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>153</x:v>
+        <x:v>156</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
         <x:v>55</x:v>

</xml_diff>

<commit_message>
Add invoke to link data entry workflow
</commit_message>
<xml_diff>
--- a/Data/Input/Test_Quote.xlsx
+++ b/Data/Input/Test_Quote.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
   <x:si>
     <x:t>Item Description</x:t>
   </x:si>
@@ -428,13 +428,10 @@
     <x:t>Units ISP Fiber Deployment- Estate Acquisition Gated Community clusters (over 2000 Units )</x:t>
   </x:si>
   <x:si>
-    <x:t>Costs</x:t>
+    <x:t>Installation of Aerial Cable</x:t>
   </x:si>
   <x:si>
-    <x:t>Service Costs</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ksh 276,804.52</x:t>
+    <x:t>43.00</x:t>
   </x:si>
   <x:si>
     <x:t>510</x:t>
@@ -443,16 +440,10 @@
     <x:t>21,930.00</x:t>
   </x:si>
   <x:si>
-    <x:t>Material costs</x:t>
+    <x:t>As built documents</x:t>
   </x:si>
   <x:si>
-    <x:t>Ksh 52,258.40</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Total Excluding VAT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Ksh 329,062.92</x:t>
+    <x:t>5.28</x:t>
   </x:si>
   <x:si>
     <x:t>397</x:t>
@@ -564,6 +555,12 @@
   </x:si>
   <x:si>
     <x:t>440.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Total Brown Field :</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ksh 275,525.16</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -30148,15 +30145,15 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:5">
+    <x:row r="1" spans="1:6">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="0" t="s">
-        <x:v>137</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C1" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="D1" s="0" t="s">
         <x:v>3</x:v>
@@ -30164,27 +30161,36 @@
       <x:c r="E1" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:5">
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6">
       <x:c r="A2" s="0" t="s">
+        <x:v>137</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
         <x:v>138</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="D2" s="0" t="s">
         <x:v>139</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
+      <x:c r="E2" s="0" t="s">
         <x:v>140</x:v>
       </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>141</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:5">
+    </x:row>
+    <x:row r="3" spans="1:6">
       <x:c r="A3" s="0" t="s">
-        <x:v>142</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>143</x:v>
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>48</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>49</x:v>
@@ -30193,191 +30199,194 @@
         <x:v>48</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:5">
+    <x:row r="4" spans="1:6">
       <x:c r="A4" s="0" t="s">
+        <x:v>141</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>142</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>143</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
         <x:v>144</x:v>
       </x:c>
-      <x:c r="B4" s="0" t="s">
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" s="0" t="s">
         <x:v>145</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>146</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="s">
-        <x:v>147</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:5">
-      <x:c r="A5" s="0" t="s">
-        <x:v>148</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>149</x:v>
+        <x:v>146</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>150</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:5">
+        <x:v>147</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6">
       <x:c r="A6" s="0" t="s">
-        <x:v>151</x:v>
+        <x:v>148</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>152</x:v>
+        <x:v>149</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>146</x:v>
+        <x:v>143</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>153</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:5">
+        <x:v>150</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:6">
       <x:c r="A7" s="0" t="s">
-        <x:v>154</x:v>
+        <x:v>151</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>155</x:v>
+        <x:v>152</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>156</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
         <x:v>97</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:5">
+    <x:row r="8" spans="1:6">
       <x:c r="A8" s="0" t="s">
-        <x:v>157</x:v>
+        <x:v>154</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>158</x:v>
+        <x:v>155</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
         <x:v>60</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>159</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:5">
+        <x:v>156</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:6">
       <x:c r="A9" s="0" t="s">
-        <x:v>160</x:v>
+        <x:v>157</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>161</x:v>
+        <x:v>158</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
         <x:v>60</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>162</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:5">
+        <x:v>159</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:6">
       <x:c r="A10" s="0" t="s">
-        <x:v>163</x:v>
+        <x:v>160</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
+        <x:v>161</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>162</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>163</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:6">
+      <x:c r="A11" s="0" t="s">
         <x:v>164</x:v>
-      </x:c>
-      <x:c r="D10" s="0" t="s">
-        <x:v>165</x:v>
-      </x:c>
-      <x:c r="E10" s="0" t="s">
-        <x:v>166</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:5">
-      <x:c r="A11" s="0" t="s">
-        <x:v>167</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>168</x:v>
+        <x:v>165</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>169</x:v>
+        <x:v>166</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>161</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:5">
+        <x:v>158</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:6">
       <x:c r="A12" s="0" t="s">
-        <x:v>170</x:v>
+        <x:v>167</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>171</x:v>
+        <x:v>168</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
+        <x:v>166</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
         <x:v>169</x:v>
       </x:c>
-      <x:c r="E12" s="0" t="s">
-        <x:v>172</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:5">
+    </x:row>
+    <x:row r="13" spans="1:6">
       <x:c r="A13" s="0" t="s">
-        <x:v>173</x:v>
+        <x:v>170</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
+        <x:v>171</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>172</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>173</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:6">
+      <x:c r="A14" s="0" t="s">
         <x:v>174</x:v>
-      </x:c>
-      <x:c r="D13" s="0" t="s">
-        <x:v>175</x:v>
-      </x:c>
-      <x:c r="E13" s="0" t="s">
-        <x:v>176</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:5">
-      <x:c r="A14" s="0" t="s">
-        <x:v>177</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>178</x:v>
+        <x:v>175</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>179</x:v>
+        <x:v>176</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>180</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:5">
+        <x:v>177</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:6">
       <x:c r="A15" s="0" t="s">
         <x:v>54</x:v>
       </x:c>
@@ -30394,7 +30403,7 @@
         <x:v>55</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:5">
+    <x:row r="16" spans="1:6">
       <x:c r="A16" s="0" t="s">
         <x:v>96</x:v>
       </x:c>
@@ -30411,7 +30420,7 @@
         <x:v>97</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:5">
+    <x:row r="17" spans="1:6">
       <x:c r="A17" s="0" t="s">
         <x:v>129</x:v>
       </x:c>
@@ -30428,21 +30437,29 @@
         <x:v>130</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:5">
+    <x:row r="18" spans="1:6">
       <x:c r="A18" s="0" t="s">
-        <x:v>181</x:v>
+        <x:v>178</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
         <x:v>47</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>182</x:v>
+        <x:v>179</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>156</x:v>
+        <x:v>153</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
         <x:v>55</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:6">
+      <x:c r="A19" s="0" t="s">
+        <x:v>180</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>181</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>